<commit_message>
Add more owner & lawyer
</commit_message>
<xml_diff>
--- a/files/buyer_template.xlsx
+++ b/files/buyer_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\skep\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEB2FD80-7609-41E1-A54F-7DBFC4A4CFFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6B77DE5-503D-4198-BDF3-82DE046688B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D1463624-6010-454E-B153-EED1864402F8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D1463624-6010-454E-B153-EED1864402F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>BIL</t>
   </si>
@@ -39,15 +39,6 @@
     <t>NO.PETAK</t>
   </si>
   <si>
-    <t>NO.PETAK AKSESORI(JIKA ADA)</t>
-  </si>
-  <si>
-    <t>KELUASAN LANTAI PETAK(SQ.M)</t>
-  </si>
-  <si>
-    <t>KELUASAN LANTAI PETAK AKSESORI(SQ.M)</t>
-  </si>
-  <si>
     <t>UNIT SHARE</t>
   </si>
   <si>
@@ -66,9 +57,6 @@
     <t>ALAMAT</t>
   </si>
   <si>
-    <t>ALAMAT SURAT MENYURAT(JIKA BERLAINAN)</t>
-  </si>
-  <si>
     <t>NO.TELEFON BIMBIT</t>
   </si>
   <si>
@@ -81,16 +69,58 @@
     <t>KEWARGANEGARAAN</t>
   </si>
   <si>
-    <t>STATUS PENGHUNIAN(PEMILIK,PENYEWA,KOSONG)</t>
-  </si>
-  <si>
-    <t>CAJ PENYENGGARAAN(RM1.89)</t>
-  </si>
-  <si>
     <t>SINKING FUND (RM)</t>
   </si>
   <si>
     <t>CATATAN</t>
+  </si>
+  <si>
+    <t>NO.KAD PENGENALAN PEMILIK 2</t>
+  </si>
+  <si>
+    <t>EMEL PEMILIK 2</t>
+  </si>
+  <si>
+    <t>NO.TELEFON BIMBIT PEMILIK 2</t>
+  </si>
+  <si>
+    <t>NAMA PEMILIK 3</t>
+  </si>
+  <si>
+    <t>NO.KAD PENGENALAN PEMILIK 3</t>
+  </si>
+  <si>
+    <t>EMEL PEMILIK 3</t>
+  </si>
+  <si>
+    <t>NO.TELEFON BIMBIT PEMILIK 3</t>
+  </si>
+  <si>
+    <t>NAMA PEGUAMCARA</t>
+  </si>
+  <si>
+    <t>ALAMAT PEGUAMCARA</t>
+  </si>
+  <si>
+    <t>NO RUJ FAIL PEGUAMCARA</t>
+  </si>
+  <si>
+    <t>CAJ PENYENGGARAAN (RM)</t>
+  </si>
+  <si>
+    <t>STATUS PENGHUNIAN (PEMILIK, PENYEWA, KOSONG)</t>
+  </si>
+  <si>
+    <t>NO.PETAK AKSESORI (JIKA ADA)</t>
+  </si>
+  <si>
+    <t>KELUASAN LANTAI PETAK (SQ.M)</t>
+  </si>
+  <si>
+    <t>KELUASAN LANTAI PETAK AKSESORI (SQ.M)</t>
+  </si>
+  <si>
+    <t>ALAMAT SURAT MENYURAT (JIKA BERLAINAN)</t>
   </si>
 </sst>
 </file>
@@ -122,24 +152,11 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -162,15 +179,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -178,7 +191,18 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -488,41 +512,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C71E4A5-768F-432E-90F2-450DD17325FC}">
-  <dimension ref="A1:W1"/>
+  <dimension ref="A1:AF1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="38.21875" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.21875" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="40.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="45.77734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="28" style="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="18.21875" style="3" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="8.88671875" style="3"/>
+    <col min="1" max="1" width="3.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="41" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="47.21875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="24.77734375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="29.21875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="27.5546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="29.21875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="27.5546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="24.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -536,25 +568,25 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>11</v>
@@ -563,37 +595,68 @@
         <v>10</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="Q1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="V1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="W1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>21</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A1:AF1">
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>